<commit_message>
done with internal radar
</commit_message>
<xml_diff>
--- a/data/Excel/指标维度库.xlsx
+++ b/data/Excel/指标维度库.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="129">
   <si>
     <t xml:space="preserve">数据名</t>
   </si>
@@ -326,12 +326,6 @@
   </si>
   <si>
     <t xml:space="preserve">医疗盈余率▲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">医务人员满意度▲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">医务人员满意度</t>
   </si>
   <si>
     <t xml:space="preserve">医院感染发生率</t>
@@ -524,11 +518,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.33"/>
@@ -1299,15 +1293,15 @@
         <v>102</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B97" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="B97" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,20 +1309,20 @@
         <v>105</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>3</v>
@@ -1336,31 +1330,31 @@
     </row>
     <row r="101" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>33</v>
@@ -1368,15 +1362,15 @@
     </row>
     <row r="105" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>10</v>
@@ -1384,47 +1378,47 @@
     </row>
     <row r="107" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>23</v>
@@ -1432,23 +1426,23 @@
     </row>
     <row r="113" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>28</v>
@@ -1456,15 +1450,15 @@
     </row>
     <row r="116" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>33</v>
@@ -1472,23 +1466,23 @@
     </row>
     <row r="118" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>33</v>
@@ -1496,20 +1490,13 @@
     </row>
     <row r="121" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B122" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>